<commit_message>
added and changed some files to send the shift that you made
</commit_message>
<xml_diff>
--- a/giovannitheproject/djsg/media/djsg/shifts/5月のShift.xlsx
+++ b/giovannitheproject/djsg/media/djsg/shifts/5月のShift.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>勤務可能日</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>中尾</t>
+  </si>
+  <si>
+    <t>石原</t>
   </si>
   <si>
     <t>出勤日</t>
@@ -475,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,100 +488,100 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="7" t="s">
+      <c r="O1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="7" t="s">
+      <c r="V1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:32">
@@ -696,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>4</v>
@@ -737,11 +740,11 @@
       <c r="S3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="T3" s="7" t="n">
-        <v>1</v>
+      <c r="T3" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="V3" s="7" t="n">
         <v>2</v>
@@ -758,23 +761,23 @@
       <c r="Z3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AA3" s="7" t="n">
-        <v>1</v>
+      <c r="AA3" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="AB3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="AC3" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD3" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE3" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF3" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:32">
@@ -791,7 +794,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>4</v>
@@ -835,11 +838,11 @@
       <c r="S4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="T4" s="7" t="s">
-        <v>4</v>
+      <c r="T4" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="V4" s="7" t="n">
         <v>1</v>
@@ -856,23 +859,23 @@
       <c r="Z4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AA4" s="7" t="s">
-        <v>4</v>
+      <c r="AA4" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="AB4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="AC4" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD4" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE4" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF4" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -886,7 +889,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>4</v>
@@ -916,7 +919,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>4</v>
@@ -958,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="AC5" s="7" t="s">
         <v>4</v>
@@ -970,6 +973,104 @@
         <v>4</v>
       </c>
       <c r="AF5" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF6" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -979,6 +1080,524 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AF7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:32">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2" t="n">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="O2" t="n">
+        <v>14</v>
+      </c>
+      <c r="P2" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>16</v>
+      </c>
+      <c r="R2" t="n">
+        <v>17</v>
+      </c>
+      <c r="S2" t="n">
+        <v>18</v>
+      </c>
+      <c r="T2" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="V2" t="n">
+        <v>21</v>
+      </c>
+      <c r="W2" t="n">
+        <v>22</v>
+      </c>
+      <c r="X2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" t="s">
+        <v>4</v>
+      </c>
+      <c r="W5" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V6" t="s">
+        <v>4</v>
+      </c>
+      <c r="W6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -993,105 +1612,105 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="n">
+      <c r="B2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="n">
+      <c r="M2" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="N2" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="T2" s="3" t="n">
+      <c r="T2" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="U2" s="2" t="n">
+      <c r="U2" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Y2" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="Z2" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AA2" s="3" t="n">
+      <c r="AA2" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="AB2" s="2" t="n">
+      <c r="AB2" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AC2" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AD2" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AE2" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2" s="4" t="n">
         <v>31</v>
       </c>
     </row>
@@ -1136,7 +1755,7 @@
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O3" t="s">
         <v>3</v>
@@ -1157,7 +1776,7 @@
         <v>3</v>
       </c>
       <c r="U3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V3" t="s">
         <v>3</v>
@@ -1178,7 +1797,7 @@
         <v>3</v>
       </c>
       <c r="AB3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC3" t="s">
         <v>3</v>
@@ -1204,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -1234,7 +1853,7 @@
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O4" t="s">
         <v>3</v>
@@ -1252,7 +1871,7 @@
         <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U4" t="s">
         <v>3</v>
@@ -1273,7 +1892,7 @@
         <v>3</v>
       </c>
       <c r="AA4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB4" t="s">
         <v>4</v>
@@ -1374,7 +1993,7 @@
         <v>3</v>
       </c>
       <c r="AB5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC5" t="s">
         <v>4</v>
@@ -1389,423 +2008,101 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:32"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AF5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:32">
-      <c r="A1" t="s">
+    <row r="6" spans="1:32">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:32">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="J2" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="K2" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="L2" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="M2" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="N2" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="O2" s="4" t="n">
-        <v>14</v>
-      </c>
-      <c r="P2" s="4" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="R2" s="4" t="n">
-        <v>17</v>
-      </c>
-      <c r="S2" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="T2" s="6" t="n">
-        <v>19</v>
-      </c>
-      <c r="U2" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="V2" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="W2" s="4" t="n">
-        <v>22</v>
-      </c>
-      <c r="X2" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="Y2" s="4" t="n">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="AA2" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="AB2" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="AC2" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="4" t="n">
-        <v>29</v>
-      </c>
-      <c r="AE2" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="AF2" s="4" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R3" t="s">
-        <v>3</v>
-      </c>
-      <c r="S3" t="s">
-        <v>3</v>
-      </c>
-      <c r="T3" t="s">
-        <v>4</v>
-      </c>
-      <c r="U3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W3" t="s">
-        <v>3</v>
-      </c>
-      <c r="X3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U4" t="s">
-        <v>4</v>
-      </c>
-      <c r="V4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W4" t="s">
-        <v>3</v>
-      </c>
-      <c r="X4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" t="s">
-        <v>4</v>
-      </c>
-      <c r="S5" t="s">
-        <v>4</v>
-      </c>
-      <c r="T5" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" t="s">
-        <v>4</v>
-      </c>
-      <c r="V5" t="s">
-        <v>4</v>
-      </c>
-      <c r="W5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF5" t="s">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V6" t="s">
+        <v>4</v>
+      </c>
+      <c r="W6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>